<commit_message>
Fix spi flash layout size
</commit_message>
<xml_diff>
--- a/board/Tiny-up5k.xlsx
+++ b/board/Tiny-up5k.xlsx
@@ -159,7 +159,7 @@
     <t>Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
-    <t>GRM188R61A106KE69D</t>
+    <t>C1608X5R1A106K080AC</t>
   </si>
   <si>
     <t>C5,C8-C11</t>
@@ -171,7 +171,7 @@
     <t>Capacitor_SMD:C_0402_1005Metric</t>
   </si>
   <si>
-    <t>GRM155R71A104KA01D</t>
+    <t>C0402C104J8RACTU</t>
   </si>
   <si>
     <t>C6,C12-C14</t>
@@ -180,7 +180,7 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>GRM155R61A103KA01D</t>
+    <t>C0402C103K8RACAUTO</t>
   </si>
   <si>
     <t>C1-C4</t>
@@ -189,7 +189,7 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>GRM155R61A105KE15D</t>
+    <t>CC0402KRX5R6BB105</t>
   </si>
   <si>
     <t>D1</t>
@@ -255,7 +255,7 @@
     <t>R2,R3</t>
   </si>
   <si>
-    <t>56</t>
+    <t>68</t>
   </si>
   <si>
     <t>CRCW040256R0FKED</t>
@@ -384,7 +384,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>do 18 okt 2018 21:22:02 CEST</t>
+    <t>wo 07 nov 2018 08:29:51 CET</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -399,7 +399,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2018-10-18 21:27:39</t>
+    <t>2018-11-07 08:31:08</t>
   </si>
   <si>
     <t>Distributors scraped by KiCost® v.1.0.3</t>

</xml_diff>